<commit_message>
fixed #391 TournRPG-391 仲間テーブルの作成
</commit_message>
<xml_diff>
--- a/docs/player.xlsx
+++ b/docs/player.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="player" sheetId="1" r:id="rId4"/>
     <sheet name="player_init" sheetId="2" r:id="rId5"/>
+    <sheet name="player_npc" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>lv</t>
   </si>
@@ -104,6 +105,39 @@
   <si>
     <t>SKILL005</t>
   </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ツユクサ</t>
+  </si>
+  <si>
+    <t>クレナイ</t>
+  </si>
+  <si>
+    <t>アイビー</t>
+  </si>
+  <si>
+    <t>アイリス</t>
+  </si>
+  <si>
+    <t>イリス</t>
+  </si>
+  <si>
+    <t>アヤメ</t>
+  </si>
+  <si>
+    <t>アオキバ</t>
+  </si>
+  <si>
+    <t>アオマツリ</t>
+  </si>
+  <si>
+    <t>アカガシ</t>
+  </si>
+  <si>
+    <t>アカシア</t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +222,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -214,6 +248,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -3861,4 +3898,310 @@
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.4141" style="10" customWidth="1"/>
+    <col min="3" max="3" width="4.17188" style="10" customWidth="1"/>
+    <col min="4" max="4" width="4.17188" style="10" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="3.17188" style="10" customWidth="1"/>
+    <col min="7" max="7" width="3.5" style="10" customWidth="1"/>
+    <col min="8" max="256" width="12" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="14.95" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="14.95" customHeight="1">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>50</v>
+      </c>
+      <c r="E3" s="8">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="14.95" customHeight="1">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>50</v>
+      </c>
+      <c r="E4" s="8">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" ht="14.95" customHeight="1">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>50</v>
+      </c>
+      <c r="E5" s="8">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="14.95" customHeight="1">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>34</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>50</v>
+      </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="14.95" customHeight="1">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>50</v>
+      </c>
+      <c r="E7" s="8">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="14.95" customHeight="1">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" ht="14.95" customHeight="1">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>50</v>
+      </c>
+      <c r="E9" s="8">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" ht="14.95" customHeight="1">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="5">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>50</v>
+      </c>
+      <c r="E10" s="8">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" ht="14.95" customHeight="1">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>50</v>
+      </c>
+      <c r="E11" s="8">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" ht="14.95" customHeight="1">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>